<commit_message>
Experiment execution      Purpose: Wideband characterization     Device: Nickel 15-60 2023-11-07     # Trials: 1
    Generation Settings:
    	Tone amplitude: 0.5
    	Duration: 1.5 seconds
    	Sampling frequency: 44100.0 Hz
    	Min Frequency: 100 Hz
    	Max frequency: 11025.0 Hz
    	Frequency spacing: 100.0 Hz
    
    Analysis Settings:
    	Fundamental frequency notch width (fraction of center frequency): 0.1
    	Fundamental frequency search width (fraction of center frequency): 0.01
    	Time ignored at beginning of recording: 0.25 seconds
    	Time ignored at end of recording: 0.25 seconds
    	Resuling DFT bin size: 1.0 Hz
    	Saturation threshold: 0.95
    	# of samples allowed at saturation threshold: 0
    	Underdrive threshold: 0.001
</commit_message>
<xml_diff>
--- a/Washer Material Code.xlsx
+++ b/Washer Material Code.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bnous\Documents\repos\measure-total-harmonic-distortion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F90BD93B-400F-4478-9C52-F80D3ADE4713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79F3AA2-1A80-45A4-B83D-2A1FFB2F8DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8CDE2132-D66A-4002-974F-31D5968A5BD5}"/>
   </bookViews>
@@ -408,9 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069BD780-83B7-44D8-BA75-C453B6B2DBD0}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -463,6 +461,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009B83433369B38544A573851AD208F122" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3981c3de111ce6271c016d9026a364b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32d83bfa-039c-4e8e-af90-17babdf74a5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1c1278cfc8c3723030037b42ab35e96b" ns3:_="">
     <xsd:import namespace="32d83bfa-039c-4e8e-af90-17babdf74a5d"/>
@@ -606,22 +619,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65865516-71D4-407F-97D5-020189B617B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="32d83bfa-039c-4e8e-af90-17babdf74a5d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE583F89-0682-4631-A79B-1D9ED3F68A2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41F52008-0427-4DF9-ACC1-3EA192094FC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -637,28 +659,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE583F89-0682-4631-A79B-1D9ED3F68A2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65865516-71D4-407F-97D5-020189B617B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="32d83bfa-039c-4e8e-af90-17babdf74a5d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>